<commit_message>
init after ignore data
</commit_message>
<xml_diff>
--- a/data/UNSD — Methodology.xlsx
+++ b/data/UNSD — Methodology.xlsx
@@ -12745,8 +12745,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100471E9650B65F724A80200CBAA92470B4" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14fe420d9e62f28664c3fd9b8d97ae55">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f15cab8-2202-4768-b37e-c47f9a7ac1c3" xmlns:ns3="1278a93a-c2fe-41ef-8498-6f29b18a37e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff381e3513c52129861e265a9b588253" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100471E9650B65F724A80200CBAA92470B4" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0d37db705df1fba950b5aa1dea2c854e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f15cab8-2202-4768-b37e-c47f9a7ac1c3" xmlns:ns3="1278a93a-c2fe-41ef-8498-6f29b18a37e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df462b4b705f6b265b1e6deb6e62f2d9" ns2:_="" ns3:_="">
     <xsd:import namespace="4f15cab8-2202-4768-b37e-c47f9a7ac1c3"/>
     <xsd:import namespace="1278a93a-c2fe-41ef-8498-6f29b18a37e3"/>
     <xsd:element name="properties">
@@ -12765,6 +12765,7 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -12818,6 +12819,13 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="f5f3f4cc-79b9-4d17-b8fa-dd7577b1fbe8" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1278a93a-c2fe-41ef-8498-6f29b18a37e3" elementFormDefault="qualified">
@@ -12959,7 +12967,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B254FF8-066C-4DE0-B59D-9F89AB806A93}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3BD08A6-966E-41A1-9490-439555CCB2F9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>